<commit_message>
changed factor as rolling mean / rolling std
</commit_message>
<xml_diff>
--- a/data/calibration_parameters.xlsx
+++ b/data/calibration_parameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>calibration-parameters</t>
   </si>
@@ -31,16 +31,13 @@
     <t>t_past</t>
   </si>
   <si>
-    <t>scale</t>
-  </si>
-  <si>
     <t>window</t>
   </si>
   <si>
     <t>^GSPC</t>
   </si>
   <si>
-    <t>2021-11-26</t>
+    <t>2021-12-14</t>
   </si>
 </sst>
 </file>
@@ -398,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,7 +411,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -422,7 +419,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -430,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4701.4599609375</v>
+        <v>4668.97021484375</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -446,14 +443,6 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
setting params to well working case study
</commit_message>
<xml_diff>
--- a/data/calibration_parameters.xlsx
+++ b/data/calibration_parameters.xlsx
@@ -37,7 +37,7 @@
     <t>^GSPC</t>
   </si>
   <si>
-    <t>2021-12-24</t>
+    <t>2022-01-03</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4725.7900390625</v>
+        <v>4766.18017578125</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>

<commit_message>
integrated old case study
</commit_message>
<xml_diff>
--- a/data/calibration_parameters.xlsx
+++ b/data/calibration_parameters.xlsx
@@ -34,10 +34,10 @@
     <t>window</t>
   </si>
   <si>
-    <t>^GSPC</t>
-  </si>
-  <si>
-    <t>2022-01-03</t>
+    <t>WTI</t>
+  </si>
+  <si>
+    <t>2019-01-07</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4766.18017578125</v>
+        <v>48.27</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>